<commit_message>
Comparación de modelos por enfermedad entrenada individual, conjunta y globalmente
</commit_message>
<xml_diff>
--- a/predictions/multiple/Enfermedades cardíacas.xlsx
+++ b/predictions/multiple/Enfermedades cardíacas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>R2</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -457,10 +462,15 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5434116749034422</v>
+        <v>0.5256126682387602</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9891795195520867</v>
+        <v>0.9895339355731295</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>multiple</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -470,10 +480,15 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2497942534858315</v>
+        <v>0.235593565623943</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9951177650337653</v>
+        <v>0.9953953178351463</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>multiple</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -483,10 +498,15 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2790136535020786</v>
+        <v>0.2782160958434385</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9946323977329595</v>
+        <v>0.9946477409688294</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>multiple</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -496,10 +516,15 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4152309245252825</v>
+        <v>0.41252899801167</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9918122146701844</v>
+        <v>0.9918654929617656</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>multiple</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>